<commit_message>
Replaced document with new version
</commit_message>
<xml_diff>
--- a/01_【09_JISA】別添1_本システムで検証を行うデータ及びデータのやり取りの内容.xlsx
+++ b/01_【09_JISA】別添1_本システムで検証を行うデータ及びデータのやり取りの内容.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26219"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\efiles\工業会証明書デジタル化コンソーシアム\70_成果物の作成\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\efiles\工業会証明書デジタル化コンソーシアム\100_納入成果物\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4CD95A-EF63-4732-BE8D-73CC4D33AEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE779D2B-50FC-4CB8-95BF-B3A7E78B3B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="180" windowWidth="15150" windowHeight="10230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="1365" windowWidth="19200" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="本システムで検証を行うデータ及びデータのやり取りの内容" sheetId="2" r:id="rId1"/>
-    <sheet name="資料②" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,37 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
-  <si>
-    <t>（別添資料）本システムで検証を行うデータ及びデータのやり取りの内容</t>
-    <rPh sb="1" eb="3">
-      <t>ベッテン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>シリョウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>何を</t>
     <rPh sb="0" eb="1">
       <t>ナニ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>誰が</t>
     <rPh sb="0" eb="1">
       <t>ダレ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>誰に</t>
     <rPh sb="0" eb="1">
       <t>ダレ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>誰が発行した</t>
@@ -77,15 +66,15 @@
     <rPh sb="2" eb="4">
       <t>ハッコウ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>どこで</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>storageにアクセス可能な人は誰で、どのようにアクセス制御をするのか</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>課題の対象</t>
@@ -95,7 +84,7 @@
     <rPh sb="3" eb="5">
       <t>タイショウ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>要検証な課題（データや相手方の検証）</t>
@@ -105,11 +94,11 @@
     <rPh sb="15" eb="17">
       <t>ケンショウ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>検証対象</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>検証方式</t>
@@ -123,7 +112,7 @@
     <rPh sb="2" eb="3">
       <t>シャ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>データの保有者
@@ -131,7 +120,7 @@
     <rPh sb="4" eb="7">
       <t>ホユウシャ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>発行者
@@ -139,7 +128,7 @@
     <rPh sb="0" eb="3">
       <t>ハッコウシャ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>データの置き場所
@@ -153,12 +142,12 @@
     <rPh sb="7" eb="8">
       <t>ショ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>アクセスコントロール
 (access control)</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>成果・留意点</t>
@@ -199,7 +188,7 @@
     <rPh sb="21" eb="23">
       <t xml:space="preserve">ケンショウ </t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t xml:space="preserve">①中小事業者等
@@ -213,7 +202,7 @@
     <rPh sb="5" eb="6">
       <t xml:space="preserve">ナド </t>
     </rPh>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>①中小事業者</t>
@@ -224,13 +213,13 @@
   </si>
   <si>
     <t>・当UCにおいてStorageにアクセス可能なアクターは、中小事業者及び中小事業者の従業員となり、事業者VCを以てStorageへのアクセスのコントロールを行う</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>・「事業者VC」について、申請者が本当に在籍しているかを検証可能となる所属証明情報(在籍確認日、在籍確認手法)を追加する
 ・GビズIDは現状、民間解放がされていない為、DNSとDIDのバインディングを前提とすることで確からしさを確保する。
 ・VCのやりとりには「トランザクションID」、VC同士の紐づきには「認証番号」を追加することで、それぞれをトレーサブルにする。</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>②事業者が用いているソフトウエアの内容 [SW利用VC]
@@ -288,7 +277,7 @@
   <si>
     <t>＜証明書申請者＞
 中小事業者</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -339,7 +328,7 @@
   <si>
     <t>＜証明書要求者＞
 全国のIT企業等の設備メーカー等</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>証明書の真正性に関わる確認や、根拠に関わる確認などで、代表団体等の工業会からの疑義発生時の照会応対の必要性がなくなること。</t>
@@ -353,7 +342,7 @@
   <si>
     <t>＜証明書提供者＞
 代表団体等の工業会等（証明団体として指定団体）</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>申請内容の真正性に係る確認コストの低減。</t>
@@ -381,7 +370,7 @@
     <t>＜証明書検証者　兼　証明書提供者＞
 所管官庁（中小企業庁）
  </t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>現状では各工業会から月次で設備種目別の交付枚数の報告を受けるに留まり、設備投資に係るデータを把握できていない（別途調査を外注）。</t>
@@ -402,7 +391,7 @@
   <si>
     <t>＜証明書検証者＞
 所轄の税務署</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t> 確定申告の内容の真正性に係る確認コストの低減。</t>
@@ -424,24 +413,18 @@
 所管官庁(当該中小事業者の業種所管)</t>
   </si>
   <si>
-    <t>■資料②</t>
+    <t>（別添１）本システムで検証を行うデータ及びデータのやり取りの内容</t>
     <rPh sb="1" eb="3">
-      <t>シリョウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>左記の4種の証明書自身と、証明書の発行者の検証</t>
-  </si>
-  <si>
-    <t>・当UCにおいてStorageにアクセス可能なアクターは、中小事業者及び中小事業者の従業員となり、事業者VCを以てStorageへのアクセスのコントロールを行う</t>
+      <t>ベッテン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,7 +442,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="游ゴシック"/>
@@ -468,39 +457,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
-      <name val="游ゴシック"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="メイリオ"/>
@@ -509,33 +465,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
     </font>
     <font>
       <b/>
@@ -562,14 +495,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Meiryo UI"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
       <family val="3"/>
@@ -622,10 +547,24 @@
       <sz val="12"/>
       <color rgb="FF444444"/>
       <name val="Meiryo UI"/>
-      <charset val="1"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,18 +584,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -722,15 +655,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -804,261 +728,219 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1341,374 +1223,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABFC499-46ED-4C5E-B26C-B44DE9D6C965}">
-  <dimension ref="A1:K25"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.25" style="23" customWidth="1"/>
-    <col min="3" max="3" width="66" style="17" customWidth="1"/>
-    <col min="4" max="4" width="39.125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="27.125" style="17" customWidth="1"/>
-    <col min="6" max="7" width="15.125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="26.625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="23.125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="49.5" style="17" customWidth="1"/>
-    <col min="11" max="11" width="44.875" style="17" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="2"/>
+    <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.25" style="8" customWidth="1"/>
+    <col min="3" max="3" width="66" style="6" customWidth="1"/>
+    <col min="4" max="4" width="39.125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="27.125" style="6" customWidth="1"/>
+    <col min="6" max="7" width="15.125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="26.625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="23.125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="49.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="44.875" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="35" customFormat="1" ht="18.600000000000001">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:11" s="20" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" s="70" customFormat="1" ht="31.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-    </row>
-    <row r="2" spans="1:11" ht="30">
-      <c r="A2" s="3"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="69"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="21"/>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="34.9" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="F3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="G3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="H3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="I3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="J3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="K3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="29" t="s">
+    </row>
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="258" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="44" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="12" customFormat="1" ht="258" hidden="1" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="70" t="s">
+      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="F4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="G4" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="H4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="I4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="J4" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="K4" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="62" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="268.14999999999998" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="13"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="268.14999999999998" hidden="1" customHeight="1">
-      <c r="B5" s="28"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="24" t="s">
+      <c r="E5" s="46"/>
+      <c r="F5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="41" t="s">
+      <c r="G5" s="46"/>
+      <c r="H5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="41" t="s">
+      <c r="I5" s="46"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="55"/>
+    </row>
+    <row r="6" spans="1:11" ht="108.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="13"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="62"/>
-    </row>
-    <row r="6" spans="1:11" ht="108.75" hidden="1" customHeight="1">
-      <c r="B6" s="28"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="25" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="41" t="s">
+      <c r="G6" s="46"/>
+      <c r="H6" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="41" t="s">
+      <c r="I6" s="46"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="55"/>
+    </row>
+    <row r="7" spans="1:11" ht="104.25" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="13"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="62"/>
-    </row>
-    <row r="7" spans="1:11" ht="104.25" hidden="1" customHeight="1">
-      <c r="B7" s="28"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="31" t="s">
+      <c r="E7" s="47"/>
+      <c r="F7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="59"/>
-      <c r="F7" s="42" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="42" t="s">
+      <c r="I7" s="47"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="56"/>
+    </row>
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="59"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="63"/>
-    </row>
-    <row r="8" spans="1:11" s="23" customFormat="1" ht="99" customHeight="1">
-      <c r="B8" s="69" t="s">
+      <c r="C8" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="D8" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="E8" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="64" t="s">
+      <c r="F8" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="G8" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="68" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="64" t="s">
+      <c r="J8" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="64" t="s">
+      <c r="K8" s="57"/>
+    </row>
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="41"/>
+      <c r="C9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K8" s="54"/>
-    </row>
-    <row r="9" spans="1:11" s="23" customFormat="1" ht="99" customHeight="1">
-      <c r="B9" s="69"/>
-      <c r="C9" s="32" t="s">
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="10" spans="1:11" s="8" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="41"/>
+      <c r="C10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="55"/>
-    </row>
-    <row r="10" spans="1:11" s="23" customFormat="1" ht="99" customHeight="1">
-      <c r="B10" s="69"/>
-      <c r="C10" s="32" t="s">
+      <c r="D10" s="49"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="58"/>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="55"/>
-    </row>
-    <row r="11" spans="1:11" s="23" customFormat="1" ht="64.5" customHeight="1">
-      <c r="B11" s="40" t="s">
+      <c r="C11" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="D11" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="E11" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="45" t="s">
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="44"/>
-    </row>
-    <row r="12" spans="1:11" s="23" customFormat="1" ht="159" customHeight="1">
-      <c r="B12" s="81" t="s">
+      <c r="C12" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="D12" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="E12" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="G12" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="H12" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="57"/>
+    </row>
+    <row r="13" spans="1:11" s="8" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="43"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="58"/>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="54"/>
-    </row>
-    <row r="13" spans="1:11" s="23" customFormat="1" ht="143.25" customHeight="1">
-      <c r="B13" s="82"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="55"/>
-    </row>
-    <row r="14" spans="1:11" s="23" customFormat="1" ht="210" customHeight="1">
-      <c r="B14" s="40" t="s">
+      <c r="C14" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="D14" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="79" t="s">
+      <c r="E14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="G14" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="38" t="s">
+      <c r="H14" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" spans="1:11" s="23" customFormat="1" ht="183" customHeight="1">
-      <c r="B15" s="40" t="s">
+      <c r="C15" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="D15" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="E15" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="78" t="s">
+      <c r="G15" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="H15" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="48"/>
-    </row>
-    <row r="16" spans="1:11" ht="18.75">
-      <c r="E16" s="36"/>
-    </row>
-    <row r="17" spans="5:5" ht="18" customHeight="1">
-      <c r="E17" s="36"/>
-    </row>
-    <row r="18" spans="5:5" ht="18.75">
-      <c r="E18" s="37"/>
-    </row>
-    <row r="20" spans="5:5" ht="18.75"/>
-    <row r="21" spans="5:5" ht="18.75"/>
-    <row r="22" spans="5:5" ht="18.75"/>
-    <row r="23" spans="5:5" ht="18.75"/>
-    <row r="24" spans="5:5" ht="18.75"/>
-    <row r="25" spans="5:5" ht="18.75"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="32"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="5:5" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E18" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="J4:J7"/>
@@ -1725,187 +1597,16 @@
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="J8:J15"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
-  <phoneticPr fontId="3"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18"/>
-  <cols>
-    <col min="1" max="1" width="3.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="47.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.125" style="2" customWidth="1"/>
-    <col min="5" max="8" width="15.125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="39.375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="27" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="36">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="36">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="12" customFormat="1" ht="258" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="75" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="75" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="73" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="268.14999999999998" customHeight="1">
-      <c r="B5" s="74"/>
-      <c r="C5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="73"/>
-    </row>
-    <row r="6" spans="1:10" ht="108.75" customHeight="1">
-      <c r="B6" s="74"/>
-      <c r="C6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="75"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="73"/>
-    </row>
-    <row r="7" spans="1:10" ht="104.25" customHeight="1">
-      <c r="B7" s="74"/>
-      <c r="C7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="73"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="E8" s="16"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="H4:H7"/>
-  </mergeCells>
-  <phoneticPr fontId="3"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>